<commit_message>
Add Calc_I_EST, Metric(MAE, MAPE, RMSE) and Plots DSS_EST
</commit_message>
<xml_diff>
--- a/openpy_dsse/examples/15NodeIEEE/MEAS_files/MEAS_error_DSS.xlsx
+++ b/openpy_dsse/examples/15NodeIEEE/MEAS_files/MEAS_error_DSS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\GitHub\OpenPy-DSSE\openpy_dsse\examples\15NodeIEEE\MEAS_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71246B5F-9A85-4003-8511-92718F1B5C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus_i" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,11 @@
     <sheet name="Bus_i_PMU" sheetId="3" r:id="rId3"/>
     <sheet name="Elem_ft_PMU" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bus_i!$A$1:$V$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Elem_ft!$A$1:$T$15</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -235,8 +245,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,11 +309,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -345,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,9 +395,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,6 +447,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -586,14 +640,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,7 +717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -681,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0.08122</v>
+        <v>8.1220000000000001E-2</v>
       </c>
       <c r="H2">
         <v>1.09138</v>
@@ -729,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -764,7 +820,7 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>-0.02641</v>
+        <v>-2.6409999999999999E-2</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -779,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>-0.00429</v>
+        <v>-4.2900000000000004E-3</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -788,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>-0.00438</v>
+        <v>-4.3800000000000002E-3</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -797,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -832,7 +888,7 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>-0.05365</v>
+        <v>-5.3650000000000003E-2</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -847,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>-0.00662</v>
+        <v>-6.62E-3</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -856,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>-0.00676</v>
+        <v>-6.7600000000000004E-3</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -865,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -885,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>-0.03059</v>
+        <v>-3.0589999999999999E-2</v>
       </c>
       <c r="H5">
         <v>0.92396</v>
@@ -900,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0.04327</v>
+        <v>4.3270000000000003E-2</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -915,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>-0.01461</v>
+        <v>-1.461E-2</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -924,7 +980,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>-0.0149</v>
+        <v>-1.49E-2</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -933,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -983,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>-0.0039</v>
+        <v>-3.8999999999999998E-3</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -992,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>-0.00398</v>
+        <v>-3.98E-3</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -1001,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1048,10 +1104,10 @@
         <v>1</v>
       </c>
       <c r="P7">
-        <v>0.26172</v>
+        <v>0.26172000000000001</v>
       </c>
       <c r="Q7">
-        <v>-0.008829999999999999</v>
+        <v>-8.8299999999999993E-3</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1060,7 +1116,7 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>-0.009010000000000001</v>
+        <v>-9.0100000000000006E-3</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -1069,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1119,7 +1175,7 @@
         <v>-0.11418</v>
       </c>
       <c r="Q8">
-        <v>-0.00391</v>
+        <v>-3.9100000000000003E-3</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1128,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>-0.00399</v>
+        <v>-3.9899999999999996E-3</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1137,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1184,10 +1240,10 @@
         <v>1</v>
       </c>
       <c r="P9">
-        <v>0.04786</v>
+        <v>4.786E-2</v>
       </c>
       <c r="Q9">
-        <v>-0.01467</v>
+        <v>-1.4670000000000001E-2</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1196,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>-0.01497</v>
+        <v>-1.4970000000000001E-2</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1205,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1252,10 +1308,10 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>-0.03741</v>
+        <v>-3.7409999999999999E-2</v>
       </c>
       <c r="Q10">
-        <v>-0.01348</v>
+        <v>-1.3480000000000001E-2</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1264,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>-0.01375</v>
+        <v>-1.375E-2</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -1273,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1320,10 +1376,10 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>0.21932</v>
+        <v>0.21931999999999999</v>
       </c>
       <c r="Q11">
-        <v>-0.008540000000000001</v>
+        <v>-8.5400000000000007E-3</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -1332,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <v>-0.008710000000000001</v>
+        <v>-8.7100000000000007E-3</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -1341,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1388,10 +1444,10 @@
         <v>1</v>
       </c>
       <c r="P12">
-        <v>-0.30902</v>
+        <v>-0.30902000000000002</v>
       </c>
       <c r="Q12">
-        <v>-0.00967</v>
+        <v>-9.6699999999999998E-3</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1400,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>-0.00987</v>
+        <v>-9.8700000000000003E-3</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -1409,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1456,10 +1512,10 @@
         <v>1</v>
       </c>
       <c r="P13">
-        <v>-0.04836</v>
+        <v>-4.836E-2</v>
       </c>
       <c r="Q13">
-        <v>-0.00133</v>
+        <v>-1.33E-3</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -1468,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>-0.00136</v>
+        <v>-1.3600000000000001E-3</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -1477,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1524,10 +1580,10 @@
         <v>1</v>
       </c>
       <c r="P14">
-        <v>-0.05761</v>
+        <v>-5.7610000000000001E-2</v>
       </c>
       <c r="Q14">
-        <v>-0.0066</v>
+        <v>-6.6E-3</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -1536,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <v>-0.00673</v>
+        <v>-6.7299999999999999E-3</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -1545,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1595,7 +1651,7 @@
         <v>0.17007</v>
       </c>
       <c r="Q15">
-        <v>-0.008189999999999999</v>
+        <v>-8.1899999999999994E-3</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1604,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>-0.008359999999999999</v>
+        <v>-8.3599999999999994E-3</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -1613,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1660,10 +1716,10 @@
         <v>1</v>
       </c>
       <c r="P16">
-        <v>-0.16498</v>
+        <v>-0.16497999999999999</v>
       </c>
       <c r="Q16">
-        <v>-0.01168</v>
+        <v>-1.1679999999999999E-2</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -1672,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>-0.01192</v>
+        <v>-1.192E-2</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -1682,19 +1738,22 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -1756,7 +1815,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1782,10 +1841,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>-0.008619999999999999</v>
+        <v>-8.6199999999999992E-3</v>
       </c>
       <c r="J2">
-        <v>0.12434</v>
+        <v>0.12434000000000001</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1794,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0.12738</v>
+        <v>0.12737999999999999</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1806,10 +1865,10 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>0.02914</v>
+        <v>2.9139999999999999E-2</v>
       </c>
       <c r="R2">
-        <v>0.18307</v>
+        <v>0.18307000000000001</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1818,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1880,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1942,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2004,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2030,10 +2089,10 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>-0.04389</v>
+        <v>-4.3889999999999998E-2</v>
       </c>
       <c r="J6">
-        <v>0.01094</v>
+        <v>1.094E-2</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2042,7 +2101,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0.01114</v>
+        <v>1.1140000000000001E-2</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -2066,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -2128,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -2190,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -2252,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2314,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -2376,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -2438,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -2500,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -2526,10 +2585,10 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>0.00211</v>
+        <v>2.1099999999999999E-3</v>
       </c>
       <c r="J14">
-        <v>0.00702</v>
+        <v>7.0200000000000002E-3</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -2538,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0.00716</v>
+        <v>7.1599999999999997E-3</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -2562,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -2625,19 +2684,22 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T15" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2678,7 +2740,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2698,10 +2760,10 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>-0.0011</v>
+        <v>-1.1000000000000001E-3</v>
       </c>
       <c r="H2">
-        <v>1.00828</v>
+        <v>1.0082800000000001</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2710,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.07665</v>
+        <v>7.6649999999999996E-2</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -2719,7 +2781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2760,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2801,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2842,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2883,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2924,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2965,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3006,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3047,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3088,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3129,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3170,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3211,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3252,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3299,14 +3361,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -3353,7 +3417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3400,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -3447,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -3473,10 +3537,10 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0.00114</v>
+        <v>1.14E-3</v>
       </c>
       <c r="J4">
-        <v>0.05919</v>
+        <v>5.919E-2</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -3485,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>-45.69754</v>
+        <v>-45.697539999999996</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -3494,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -3541,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -3588,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -3635,7 +3699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -3682,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -3729,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -3776,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3823,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -3870,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -3917,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -3964,7 +4028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>

</xml_diff>